<commit_message>
Added row for a 6 channel 3 switch Flap (instead of the 7th channel). Added row to show how board leds should light in different modes.
</commit_message>
<xml_diff>
--- a/QUAD/Configuration_Standards.xlsx
+++ b/QUAD/Configuration_Standards.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>INPUTS</t>
   </si>
@@ -175,13 +175,166 @@
   </si>
   <si>
     <t>Descent at position</t>
+  </si>
+  <si>
+    <t>RX CH 6 Flaps 3 Switch</t>
+  </si>
+  <si>
+    <t>Value Mid</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Leds</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Green Fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yellow OFF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Green Slow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yellow OFF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Green Slow</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yellow ON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Green Slow</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yellow Slow</t>
+    </r>
+  </si>
+  <si>
+    <t>5.bis</t>
+  </si>
+  <si>
+    <t>V. 1.1</t>
+  </si>
+  <si>
+    <t>Emile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +387,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -412,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -511,10 +687,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,9 +707,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -562,7 +747,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -632,7 +817,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -806,106 +991,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="10" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
+    <row r="1" spans="1:11" ht="18.75">
       <c r="A1" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="35">
+      <c r="I1" s="35">
         <f ca="1">TODAY()</f>
         <v>40497</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75">
-      <c r="A2" s="34"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="F3" s="37" t="s">
+    <row r="2" spans="1:11" ht="18.75">
+      <c r="A2" s="36"/>
+      <c r="H2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="35">
+        <v>40497</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18.75">
+      <c r="A3" s="34"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="G4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="10" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="13">
+    <row r="6" spans="1:11">
+      <c r="A6" s="13">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8">
-        <v>1000</v>
-      </c>
-      <c r="E5" s="8">
-        <v>2000</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="13">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="8">
@@ -914,18 +1098,19 @@
       <c r="E6" s="8">
         <v>2000</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="8">
@@ -934,18 +1119,19 @@
       <c r="E7" s="8">
         <v>2000</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="8">
@@ -954,18 +1140,19 @@
       <c r="E8" s="8">
         <v>2000</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="13">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="8">
@@ -974,26 +1161,19 @@
       <c r="E9" s="8">
         <v>2000</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="8">
@@ -1002,9 +1182,7 @@
       <c r="E10" s="8">
         <v>2000</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F10" s="8"/>
       <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1014,14 +1192,17 @@
       <c r="I10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="8">
@@ -1030,9 +1211,7 @@
       <c r="E11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1040,501 +1219,614 @@
         <v>23</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="14">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1500</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="14">
         <v>7</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9">
+      <c r="C14" s="6"/>
+      <c r="D14" s="9">
         <v>1000</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E14" s="9">
         <v>2000</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="20" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="41"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="J16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="28" t="s">
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="15"/>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="15" t="s">
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="15"/>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="10" t="s">
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="29">
+      <c r="F20" s="40"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="29">
         <v>0</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B21" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="13">
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="13">
         <v>1</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="13">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="13">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="13">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="13">
-        <v>5</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="13">
-        <v>6</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="13">
-        <v>7</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>42</v>
+        <v>5</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="13"/>
-      <c r="B27" s="5"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="13">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="19"/>
+      <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="13" t="s">
-        <v>33</v>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="13">
+        <v>7</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="13"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="13"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="13"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="8">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="13"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="14" t="s">
+      <c r="D33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="8">
+        <v>0</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1</v>
+      </c>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="13"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="15" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="10" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B39" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E39" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="29">
+      <c r="F39" s="40"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="29">
         <v>0</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B40" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C40" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="13">
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="13">
         <v>1</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="13">
-        <v>2</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="13">
-        <v>3</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="13">
-        <v>6</v>
-      </c>
-      <c r="B44" s="31" t="s">
-        <v>43</v>
+        <v>4</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="13"/>
-      <c r="B46" s="5"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="13">
+        <v>6</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>43</v>
+      </c>
       <c r="C46" s="5"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="13" t="s">
-        <v>33</v>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="13">
+        <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="13"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="13"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="18"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="13"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="8">
-        <v>0</v>
-      </c>
-      <c r="E51" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="13"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="14" t="s">
+      <c r="D52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="18"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1</v>
+      </c>
+      <c r="F53" s="18"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="13"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="18"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="G4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1547,7 +1839,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1559,7 +1851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Igor's warnings about IN07/CH8 failsave of AMP
</commit_message>
<xml_diff>
--- a/QUAD/Configuration_Standards.xlsx
+++ b/QUAD/Configuration_Standards.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>INPUTS</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>V. 1.0</t>
-  </si>
-  <si>
-    <t>Phil</t>
   </si>
   <si>
     <t>mod by</t>
@@ -329,12 +326,51 @@
   <si>
     <t>Emile</t>
   </si>
+  <si>
+    <t>V. 1.2</t>
+  </si>
+  <si>
+    <t>phil</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>added Igor's comments abut Ch8</t>
+  </si>
+  <si>
+    <t>added 5.bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoid !!! </t>
+  </si>
+  <si>
+    <t>7 *)</t>
+  </si>
+  <si>
+    <t>*)</t>
+  </si>
+  <si>
+    <t>Avoid IN7 (Ch8)! Please read this:</t>
+  </si>
+  <si>
+    <t>http://www.rcgroups.com/forums/showpost.php?p=16561514&amp;postcount=2264</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>initial file</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +446,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -588,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,12 +716,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,19 +734,38 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -707,9 +773,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -747,7 +813,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -817,7 +883,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -991,13 +1057,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -1010,86 +1076,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="35">
-        <f ca="1">TODAY()</f>
-        <v>40497</v>
-      </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="18.75">
+      <c r="A2" s="34"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="G3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75">
-      <c r="A2" s="36"/>
-      <c r="H2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="35">
-        <v>40497</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18.75">
-      <c r="A3" s="34"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="G4" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="13">
         <v>0</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>51</v>
-      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="8">
@@ -1102,15 +1164,15 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="8">
@@ -1128,10 +1190,10 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="8">
@@ -1149,10 +1211,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="8">
@@ -1162,18 +1224,26 @@
         <v>2000</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="8">
@@ -1187,22 +1257,22 @@
         <v>23</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="13">
-        <v>5</v>
+      <c r="A11" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="8">
@@ -1211,7 +1281,9 @@
       <c r="E11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>1500</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1224,14 +1296,16 @@
       <c r="J11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="13" t="s">
-        <v>61</v>
+      <c r="A12" s="13">
+        <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="8">
@@ -1240,9 +1314,7 @@
       <c r="E12" s="8">
         <v>2000</v>
       </c>
-      <c r="F12" s="8">
-        <v>1500</v>
-      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1250,175 +1322,170 @@
         <v>23</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="13">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="15"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2000</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E14" s="9">
-        <v>2000</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="K15" s="41"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="15"/>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="19"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="40"/>
+      <c r="A20" s="29">
+        <v>0</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="45" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="29">
-        <v>0</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1426,13 +1493,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -1440,86 +1507,131 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="13">
-        <v>3</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="18"/>
+      <c r="G24" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="50"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="13">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="18"/>
+      <c r="G25" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="47">
+        <v>40496</v>
+      </c>
+      <c r="I25" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="41" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="13">
-        <v>5</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="G26" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="47">
+        <v>40497</v>
+      </c>
+      <c r="I26" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="41" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="G27" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="47">
+        <v>40498</v>
+      </c>
+      <c r="I27" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="41" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="13">
-        <v>7</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A28" s="13"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="41"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="13"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>37</v>
@@ -1530,217 +1642,241 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="18"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A31" s="13"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="18"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="13"/>
+      <c r="A32" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>24</v>
+      <c r="D33" s="8">
+        <v>0</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
       </c>
       <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="13"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="8">
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="29">
         <v>0</v>
       </c>
-      <c r="E34" s="8">
+      <c r="B39" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="13">
         <v>1</v>
       </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="13"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="40"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="29">
-        <v>0</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
+      <c r="B40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
       <c r="F40" s="18"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:10">
       <c r="A41" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="18"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:10">
       <c r="A42" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:10">
       <c r="A43" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="18"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:10">
       <c r="A44" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:10">
       <c r="A45" s="13">
-        <v>5</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>46</v>
+        <v>6</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="18"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:10">
       <c r="A46" s="13">
-        <v>6</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>43</v>
+        <v>7</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="18"/>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="13">
-        <v>7</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>42</v>
-      </c>
+    <row r="47" spans="1:10">
+      <c r="A47" s="13"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="18"/>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="13"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+    <row r="48" spans="1:10">
+      <c r="A48" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>37</v>
@@ -1753,80 +1889,66 @@
       <c r="F49" s="18"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A50" s="13"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="13"/>
+      <c r="A51" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="D51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>24</v>
+      <c r="D52" s="8">
+        <v>0</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1</v>
       </c>
       <c r="F52" s="18"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A53" s="13"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
-      <c r="D53" s="8">
-        <v>0</v>
-      </c>
-      <c r="E53" s="8">
-        <v>1</v>
-      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="18"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="13"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="A54" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
       <c r="F54" s="18"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1839,7 +1961,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1851,7 +1973,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>